<commit_message>
Deleted all useless named range
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
@@ -15,7 +15,6 @@
     <definedName name="FuturesDates">MainChecks!$C$16:$C$19</definedName>
     <definedName name="FuturesTable">MainChecks!$A$4:$H$14</definedName>
     <definedName name="IMMFutures">MainChecks!$D$16:$D$19</definedName>
-    <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
@@ -815,24 +814,22 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 09:28:42</v>
+        <v>Updated at 14:51:00</v>
         <stp/>
-        <stp>{F884A349-5DBA-44A4-A4C8-EB715CB4E960}</stp>
-        <tr r="P6" s="2"/>
+        <stp>{8ED48A2E-F766-4FFF-B1C5-E2A56410B046}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 09:31:05</v>
+        <v>Updated at 14:57:55</v>
         <stp/>
-        <stp>{2EE1AE43-4443-4FFE-A2FF-0DD99F948CDF}</stp>
+        <stp>{D3CA486E-422E-4E6A-9AD1-703455BA4EE3}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:23:51</v>
+        <v>Updated at 14:57:10</v>
         <stp/>
-        <stp>{AB1AAB78-A1F2-45F3-877E-167AB99F36FC}</stp>
-        <tr r="Q6" s="2"/>
+        <stp>{C219B1F8-DA81-475D-945C-2A3CEC07FB78}</stp>
+        <tr r="P6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1318,7 +1315,9 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="18">
+        <v>42181.618726851855</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1477,17 +1476,17 @@
         <v>FGBLc1</v>
       </c>
       <c r="L5" s="25">
-        <v>42163</v>
+        <v>42255</v>
       </c>
       <c r="M5" s="26">
-        <v>153.45000000000002</v>
+        <v>150.05000000000001</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 09:31:05</v>
+        <v>Updated at 14:57:55</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1498,7 +1497,7 @@
       </c>
       <c r="U5" s="11" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_57 / 1.6.0 / 1.6</v>
+        <v>1_58 / 1.6.0 / 1.7</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1548,25 +1547,25 @@
         <v>SEKAB3S10Y</v>
       </c>
       <c r="L6" s="22">
-        <v>42137</v>
+        <v>42181</v>
       </c>
       <c r="M6" s="30" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>1.3525/1.4025</v>
+        <v>1.655/1.705</v>
       </c>
       <c r="N6" s="28">
-        <v>1.3525</v>
+        <v>1.655</v>
       </c>
       <c r="O6" s="28">
-        <v>1.4025000000000001</v>
+        <v>1.7050000000000001</v>
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 09:28:42</v>
+        <v>Updated at 14:57:10</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 09:23:51</v>
+        <v>Updated at 14:51:00</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1577,7 +1576,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>672</v>
+        <v>770</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1750,11 +1749,11 @@
       </c>
       <c r="L9" s="57">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42136</v>
+        <v>42180</v>
       </c>
       <c r="M9" s="58">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>-1.9400000000000001E-3</v>
+        <v>-2.0600000000000002E-3</v>
       </c>
       <c r="N9" s="58"/>
       <c r="O9" s="58"/>
@@ -1816,19 +1815,19 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>SEKSTD</v>
       </c>
-      <c r="L10" s="22" t="e">
+      <c r="L10" s="22">
         <f>_xll.qlTermStructureReferenceDate(K10,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M10" s="23" t="e">
+        <v>42181</v>
+      </c>
+      <c r="M10" s="23">
         <f>_xll.qlYieldTSDiscount(K10,L10)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="31" t="str">
-        <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
+        <f>IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
         <v/>
       </c>
       <c r="R10" s="8" t="s">
@@ -1886,7 +1885,7 @@
       </c>
       <c r="L11" s="22">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>42142</v>
+        <v>42184</v>
       </c>
       <c r="M11" s="23">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
@@ -1936,19 +1935,19 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>SEK1M</v>
       </c>
-      <c r="L12" s="22" t="e">
+      <c r="L12" s="22">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M12" s="23" t="e">
+        <v>42184</v>
+      </c>
+      <c r="M12" s="23">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="32" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v/>
       </c>
       <c r="R12" s="8" t="s">
@@ -2004,19 +2003,19 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>SEK3M</v>
       </c>
-      <c r="L13" s="22" t="e">
+      <c r="L13" s="22">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M13" s="23" t="e">
+        <v>42184</v>
+      </c>
+      <c r="M13" s="23">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="32" t="str">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
@@ -2066,19 +2065,19 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>SEK6M</v>
       </c>
-      <c r="L14" s="40" t="e">
+      <c r="L14" s="40">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M14" s="41" t="e">
+        <v>42184</v>
+      </c>
+      <c r="M14" s="41">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N14" s="41"/>
       <c r="O14" s="41"/>
       <c r="P14" s="41"/>
       <c r="Q14" s="42" t="str">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v/>
       </c>
       <c r="R14" s="8" t="s">
@@ -2150,11 +2149,11 @@
       </c>
       <c r="C16" s="33">
         <f t="array" ref="C16:C19">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B16:B19)</f>
-        <v>42172</v>
+        <v>42263</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="array" ref="D16:D19">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>-M5</v>
+        <v>-U5</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2195,10 +2194,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="34">
-        <v>42263</v>
+        <v>42354</v>
       </c>
       <c r="D17" s="8" t="str">
-        <v>-U5</v>
+        <v>-Z5</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2239,10 +2238,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="34">
-        <v>42354</v>
+        <v>42445</v>
       </c>
       <c r="D18" s="8" t="str">
-        <v>-Z5</v>
+        <v>-H6</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2283,10 +2282,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="35">
-        <v>42445</v>
+        <v>42536</v>
       </c>
       <c r="D19" s="10" t="str">
-        <v>-H6</v>
+        <v>-M6</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -5476,7 +5475,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5496,12 +5495,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5521,7 +5520,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>